<commit_message>
upload open-air results v2
</commit_message>
<xml_diff>
--- a/experimental-dat/open-air-radio-test/open-air-radio-test.xlsx
+++ b/experimental-dat/open-air-radio-test/open-air-radio-test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Documents\University\Academics\4th Year Project\Radio Tests\experimental-dat\open-field-radio-test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Documents\University\Academics\4th Year Project\Radio Tests\experimental-dat\open-air-radio-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{539F837E-30DD-484A-A294-0E254D6FFCE5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{539F837E-30DD-484A-A294-0E254D6FFCE5}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -221,10 +221,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$A$2:$A$38</c:f>
+              <c:f>data!$A$2:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -334,6 +334,9 @@
                   <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>370</c:v>
                 </c:pt>
               </c:numCache>
@@ -341,10 +344,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$B$2:$B$38</c:f>
+              <c:f>data!$B$2:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -432,7 +435,7 @@
                 <c:pt idx="35">
                   <c:v>0.51</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>0.93</c:v>
                 </c:pt>
               </c:numCache>
@@ -477,10 +480,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$A$2:$A$38</c:f>
+              <c:f>data!$A$2:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -590,6 +593,9 @@
                   <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>370</c:v>
                 </c:pt>
               </c:numCache>
@@ -597,10 +603,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$C$2:$C$38</c:f>
+              <c:f>data!$C$2:$C$39</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -688,7 +694,7 @@
                 <c:pt idx="35">
                   <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>0.04</c:v>
                 </c:pt>
               </c:numCache>
@@ -1139,10 +1145,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$A$2:$A$38</c:f>
+              <c:f>data!$A$2:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1252,6 +1258,9 @@
                   <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>370</c:v>
                 </c:pt>
               </c:numCache>
@@ -1259,10 +1268,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$D$2:$D$38</c:f>
+              <c:f>data!$D$2:$D$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>11.494999999999999</c:v>
                 </c:pt>
@@ -1350,7 +1359,7 @@
                 <c:pt idx="35">
                   <c:v>11.661</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>11.728</c:v>
                 </c:pt>
               </c:numCache>
@@ -1395,10 +1404,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>data!$A$2:$A$38</c:f>
+              <c:f>data!$A$2:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1508,6 +1517,9 @@
                   <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="36">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>370</c:v>
                 </c:pt>
               </c:numCache>
@@ -1515,10 +1527,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$E$2:$E$38</c:f>
+              <c:f>data!$E$2:$E$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
                   <c:v>11.41</c:v>
                 </c:pt>
@@ -1606,7 +1618,7 @@
                 <c:pt idx="35">
                   <c:v>11.656000000000001</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="37">
                   <c:v>11.635999999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -3595,10 +3607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96ADDCF-9371-4E9E-9CF2-F3C3079A4C70}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4192,18 +4204,23 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39">
         <v>370</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B39" s="4">
         <v>0.93</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C39" s="4">
         <v>0.04</v>
       </c>
-      <c r="D38">
+      <c r="D39">
         <v>11.728</v>
       </c>
-      <c r="E38">
+      <c r="E39">
         <v>11.635999999999999</v>
       </c>
     </row>
@@ -4218,7 +4235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CBE94C-95C7-4C9E-AD55-E797540ECD38}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
       <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
( - ) sign left out of dBm measurement
</commit_message>
<xml_diff>
--- a/experimental-dat/open-air-radio-test/open-air-radio-test.xlsx
+++ b/experimental-dat/open-air-radio-test/open-air-radio-test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{539F837E-30DD-484A-A294-0E254D6FFCE5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{539F837E-30DD-484A-A294-0E254D6FFCE5}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -3207,7 +3207,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
-            <a:t>2.4GHz interference &lt;95 dBm average</a:t>
+            <a:t>2.4GHz interference &lt;-95 dBm average</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3609,7 +3609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96ADDCF-9371-4E9E-9CF2-F3C3079A4C70}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -4235,7 +4235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CBE94C-95C7-4C9E-AD55-E797540ECD38}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+    <sheetView topLeftCell="O29" workbookViewId="0">
       <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>

</xml_diff>